<commit_message>
Adding Fixed Starting Point Mechanism
</commit_message>
<xml_diff>
--- a/Datasource/Master Data - Copy.xlsx
+++ b/Datasource/Master Data - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Scenes Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="109">
   <si>
     <t>Location</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>WAWAN, MANTO, MALI, IRAH, RITA, NINA, KAKEK TUA</t>
   </si>
 </sst>
 </file>
@@ -425,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -459,10 +465,13 @@
     <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,14 +779,14 @@
   </sheetPr>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.42578125" style="11" bestFit="1" customWidth="1"/>
@@ -787,7 +796,7 @@
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -807,87 +816,87 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>9</v>
+      <c r="B2" s="12">
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10">
-        <v>-0.40765299999999999</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="F2" s="10">
-        <v>116.972959</v>
+        <v>116.973714</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1"/>
+      <c r="B3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="10">
-        <v>-0.41477399999999998</v>
+        <v>-0.40765299999999999</v>
       </c>
       <c r="F3" s="10">
-        <v>116.638374</v>
+        <v>116.972959</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>11</v>
+      <c r="B4" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="E4" s="10">
+        <v>-0.41477399999999998</v>
+      </c>
+      <c r="F4" s="10">
+        <v>116.638374</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="B5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="10">
-        <v>-0.41471000000000002</v>
-      </c>
-      <c r="F5" s="10">
-        <v>116.638901</v>
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>13</v>
+      <c r="B6" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -903,20 +912,20 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="12">
-        <v>3</v>
+      <c r="B7" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>54</v>
+        <v>4</v>
+      </c>
+      <c r="E7" s="10">
+        <v>-0.41471000000000002</v>
       </c>
       <c r="F7" s="10">
-        <v>116.973714</v>
+        <v>116.638901</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -924,7 +933,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>50</v>
@@ -943,7 +952,7 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="14">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1003,7 +1012,7 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1023,7 +1032,7 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1043,7 +1052,7 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="14">
         <v>8</v>
       </c>
       <c r="C14" s="1"/>
@@ -1061,7 +1070,7 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1081,7 +1090,7 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1101,7 +1110,7 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="14">
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1121,7 +1130,7 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="14">
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1141,7 +1150,7 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1161,51 +1170,51 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="12">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="10">
-        <v>-0.41477399999999998</v>
-      </c>
-      <c r="F20" s="10">
-        <v>116.638374</v>
+      <c r="B20" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7">
+        <v>-0.39484999999999998</v>
+      </c>
+      <c r="F20" s="7">
+        <v>117.002008</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>21</v>
+      <c r="B21" s="14">
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="10">
-        <v>-0.40765299999999999</v>
+        <v>-0.41477399999999998</v>
       </c>
       <c r="F21" s="10">
-        <v>116.972959</v>
+        <v>116.638374</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>22</v>
+      <c r="B22" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -1221,31 +1230,31 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="12">
-        <v>15</v>
+      <c r="B23" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E23" s="10">
-        <v>-0.40334300000000001</v>
+        <v>-0.40765299999999999</v>
       </c>
       <c r="F23" s="10">
-        <v>116.997378</v>
+        <v>116.972959</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>23</v>
+      <c r="B24" s="14">
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>6</v>
@@ -1261,11 +1270,11 @@
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>24</v>
+      <c r="B25" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
@@ -1281,11 +1290,11 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>25</v>
+      <c r="B26" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
@@ -1301,11 +1310,11 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>26</v>
+      <c r="B27" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
@@ -1321,11 +1330,11 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="12">
-        <v>17</v>
+      <c r="B28" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
@@ -1341,11 +1350,11 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="12">
-        <v>18</v>
+      <c r="B29" s="14">
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>6</v>
@@ -1361,30 +1370,33 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="12">
-        <v>19</v>
+      <c r="B30" s="14">
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E30" s="10">
-        <v>-0.41477399999999998</v>
+        <v>-0.40334300000000001</v>
       </c>
       <c r="F30" s="10">
-        <v>116.638374</v>
+        <v>116.997378</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="B31" s="14">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="10">
@@ -1398,48 +1410,45 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="12">
-        <v>20</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>7</v>
+      <c r="B32" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="E32" s="10">
-        <v>-0.401028</v>
+        <v>-0.41477399999999998</v>
       </c>
       <c r="F32" s="10">
-        <v>116.99877499999999</v>
+        <v>116.638374</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>27</v>
+      <c r="B33" s="14">
+        <v>20</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E33" s="10">
-        <v>-0.40765299999999999</v>
+        <v>-0.401028</v>
       </c>
       <c r="F33" s="10">
-        <v>116.972959</v>
+        <v>116.99877499999999</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>28</v>
+      <c r="B34" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>69</v>
@@ -1458,10 +1467,12 @@
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="1"/>
+      <c r="B35" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1476,8 +1487,8 @@
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>30</v>
+      <c r="B36" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
@@ -1494,28 +1505,26 @@
       <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="B37" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="10">
-        <v>-0.41477399999999998</v>
+        <v>-0.40765299999999999</v>
       </c>
       <c r="F37" s="10">
-        <v>116.638374</v>
+        <v>116.972959</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>32</v>
+      <c r="B38" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>70</v>
@@ -1534,11 +1543,11 @@
       <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>33</v>
+      <c r="B39" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>2</v>
@@ -1554,148 +1563,148 @@
       <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="12">
-        <v>24</v>
+      <c r="B40" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E40" s="10">
-        <v>-0.40334300000000001</v>
+        <v>-0.41477399999999998</v>
       </c>
       <c r="F40" s="10">
-        <v>116.997378</v>
+        <v>116.638374</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="12">
-        <v>25</v>
+      <c r="B41" s="14">
+        <v>24</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="10">
-        <v>-0.401028</v>
+        <v>-0.40334300000000001</v>
       </c>
       <c r="F41" s="10">
-        <v>116.99877499999999</v>
+        <v>116.997378</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="12">
-        <v>26</v>
+      <c r="B42" s="14">
+        <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E42" s="10">
-        <v>-0.40334300000000001</v>
+        <v>-0.401028</v>
       </c>
       <c r="F42" s="10">
-        <v>116.997378</v>
+        <v>116.99877499999999</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="12">
-        <v>27</v>
+      <c r="B43" s="14">
+        <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E43" s="10">
-        <v>-0.401028</v>
+        <v>-0.40334300000000001</v>
       </c>
       <c r="F43" s="10">
-        <v>116.99877499999999</v>
+        <v>116.997378</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
-      <c r="B44" s="12">
-        <v>28</v>
+      <c r="B44" s="14">
+        <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E44" s="10">
-        <v>-0.40334300000000001</v>
+        <v>-0.401028</v>
       </c>
       <c r="F44" s="10">
-        <v>116.997378</v>
+        <v>116.99877499999999</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="1"/>
+      <c r="B45" s="14">
+        <v>28</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="10">
-        <v>-0.401028</v>
+        <v>-0.40334300000000001</v>
       </c>
       <c r="F45" s="10">
-        <v>116.99877499999999</v>
+        <v>116.997378</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>35</v>
+      <c r="B46" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E46" s="10">
-        <v>-0.40334300000000001</v>
+        <v>-0.401028</v>
       </c>
       <c r="F46" s="10">
-        <v>116.997378</v>
+        <v>116.99877499999999</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="B47" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
         <v>6</v>
       </c>
@@ -1710,11 +1719,11 @@
       <c r="A48" s="7">
         <v>47</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>37</v>
+      <c r="B48" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>6</v>
@@ -1730,10 +1739,12 @@
       <c r="A49" s="7">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="1"/>
+      <c r="B49" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="D49" s="1" t="s">
         <v>6</v>
       </c>
@@ -1748,51 +1759,49 @@
       <c r="A50" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="12">
-        <v>31</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="B50" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E50" s="10">
-        <v>-0.41477399999999998</v>
+        <v>-0.40334300000000001</v>
       </c>
       <c r="F50" s="10">
-        <v>116.638374</v>
+        <v>116.997378</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>39</v>
+      <c r="B51" s="14">
+        <v>31</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E51" s="10">
-        <v>-0.39484999999999998</v>
+        <v>-0.41477399999999998</v>
       </c>
       <c r="F51" s="10">
-        <v>117.002008</v>
+        <v>116.638374</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>40</v>
+      <c r="B52" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
@@ -1808,28 +1817,28 @@
       <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="12" t="s">
-        <v>41</v>
+      <c r="B53" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E53" s="10">
-        <v>-0.41477399999999998</v>
+        <v>-0.39484999999999998</v>
       </c>
       <c r="F53" s="10">
-        <v>116.638374</v>
+        <v>117.002008</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>42</v>
+      <c r="B54" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>67</v>
@@ -1848,60 +1857,60 @@
       <c r="A55" s="7">
         <v>54</v>
       </c>
-      <c r="B55" s="12">
-        <v>34</v>
+      <c r="B55" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>54</v>
+        <v>2</v>
+      </c>
+      <c r="E55" s="10">
+        <v>-0.41477399999999998</v>
       </c>
       <c r="F55" s="10">
-        <v>116.973714</v>
+        <v>116.638374</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" s="10">
-        <v>-0.41477399999999998</v>
+      <c r="B56" s="12">
+        <v>34</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="F56" s="10">
-        <v>116.638374</v>
+        <v>116.973714</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
-      <c r="B57" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>54</v>
+      <c r="B57" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="10">
+        <v>-0.41477399999999998</v>
       </c>
       <c r="F57" s="10">
-        <v>116.973714</v>
+        <v>116.638374</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1909,10 +1918,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>5</v>
@@ -1928,44 +1937,61 @@
       <c r="A59" s="7">
         <v>58</v>
       </c>
-      <c r="B59" s="12">
-        <v>36</v>
+      <c r="B59" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59" s="10">
-        <v>-0.40765299999999999</v>
+        <v>5</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="F59" s="10">
-        <v>116.972959</v>
+        <v>116.973714</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
-      <c r="B60" s="12">
+      <c r="B60" s="14">
+        <v>36</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" s="10">
+        <v>-0.40765299999999999</v>
+      </c>
+      <c r="F60" s="10">
+        <v>116.972959</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>60</v>
+      </c>
+      <c r="B61" s="12">
         <v>37</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E61" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F61" s="10">
         <v>116.973714</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
     </row>
     <row r="62" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
@@ -2296,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2331,7 @@
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2321,7 +2347,7 @@
       <c r="D1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2333,14 +2359,14 @@
         <v>59</v>
       </c>
       <c r="C2">
-        <v>600000</v>
+        <v>1250000</v>
       </c>
       <c r="D2">
         <v>45</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <f>C2/D2</f>
-        <v>13333.333333333334</v>
+        <v>27777.777777777777</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2351,14 +2377,14 @@
         <v>95</v>
       </c>
       <c r="C3">
-        <v>600000</v>
+        <v>900000</v>
       </c>
       <c r="D3">
         <v>34</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <f t="shared" ref="E3:E11" si="0">C3/D3</f>
-        <v>17647.058823529413</v>
+        <v>26470.588235294119</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,14 +2395,14 @@
         <v>96</v>
       </c>
       <c r="C4">
-        <v>600000</v>
+        <v>900000</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f t="shared" si="0"/>
-        <v>24000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2387,14 +2413,14 @@
         <v>74</v>
       </c>
       <c r="C5">
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <f t="shared" si="0"/>
-        <v>37500</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2405,14 +2431,14 @@
         <v>97</v>
       </c>
       <c r="C6">
-        <v>600000</v>
+        <v>650000</v>
       </c>
       <c r="D6">
         <v>15</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>43333.333333333336</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2423,14 +2449,14 @@
         <v>94</v>
       </c>
       <c r="C7">
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="D7">
         <v>17</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <f t="shared" si="0"/>
-        <v>35294.117647058825</v>
+        <v>23529.411764705881</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2441,14 +2467,14 @@
         <v>98</v>
       </c>
       <c r="C8">
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="D8">
         <v>9</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <f t="shared" si="0"/>
-        <v>66666.666666666672</v>
+        <v>44444.444444444445</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,14 +2485,14 @@
         <v>99</v>
       </c>
       <c r="C9">
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="D9">
         <v>12</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>33333.333333333336</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,14 +2503,14 @@
         <v>100</v>
       </c>
       <c r="C10">
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="D10">
         <v>11</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <f t="shared" si="0"/>
-        <v>54545.454545454544</v>
+        <v>36363.63636363636</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2495,14 +2521,14 @@
         <v>101</v>
       </c>
       <c r="C11">
-        <v>600000</v>
+        <v>300000</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f t="shared" si="0"/>
-        <v>200000</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>